<commit_message>
Updating script and examples
</commit_message>
<xml_diff>
--- a/job-openings-scripts/muoniverse-job-openings.xlsx
+++ b/job-openings-scripts/muoniverse-job-openings.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10201"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pizzi/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pizzi/git/MUONIVERSE/website/job-openings-scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{725A853A-3A94-2544-82BE-E468ABF50A7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{626953C9-3C8D-E141-8B45-38E13DA2CEDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3260" yWindow="2160" windowWidth="28040" windowHeight="17440" xr2:uid="{F1209A29-3667-8F47-BE66-D0C7E662ABA0}"/>
   </bookViews>
@@ -43,7 +43,7 @@
     <author>tc={3A2C8F42-915E-4B42-8C35-1087C2FD6E67}</author>
     <author>tc={0DD1F034-F3C2-6143-B5EE-4D8ACB9B94D3}</author>
     <author>tc={7B781CE5-788D-EE45-89AA-868478A6290E}</author>
-    <author>tc={86A3B50E-CB66-3648-8FB2-14FCD24209F5}</author>
+    <author>tc={803435A0-8165-0344-9437-CCA1C17B6D10}</author>
   </authors>
   <commentList>
     <comment ref="A1" authorId="0" shapeId="0" xr:uid="{D3909E3A-CF3A-6144-B66D-EC5AECD54804}">
@@ -62,7 +62,7 @@
     Please use standardized name (copy name from rows above, if one already exists)</t>
       </text>
     </comment>
-    <comment ref="C1" authorId="2" shapeId="0" xr:uid="{0DD1F034-F3C2-6143-B5EE-4D8ACB9B94D3}">
+    <comment ref="D1" authorId="2" shapeId="0" xr:uid="{0DD1F034-F3C2-6143-B5EE-4D8ACB9B94D3}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -70,20 +70,21 @@
     Short 1-line job description</t>
       </text>
     </comment>
-    <comment ref="D1" authorId="3" shapeId="0" xr:uid="{7B781CE5-788D-EE45-89AA-868478A6290E}">
+    <comment ref="E1" authorId="3" shapeId="0" xr:uid="{7B781CE5-788D-EE45-89AA-868478A6290E}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    Direct link to page with full application (and link to apply)</t>
+    Direct link to page with full application (and link to apply). If not present, the button will not be shown</t>
       </text>
     </comment>
-    <comment ref="F1" authorId="4" shapeId="0" xr:uid="{86A3B50E-CB66-3648-8FB2-14FCD24209F5}">
+    <comment ref="F1" authorId="4" shapeId="0" xr:uid="{803435A0-8165-0344-9437-CCA1C17B6D10}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    If the value is "TRUE", it will not be shown on the website</t>
+    When the date is in the past, the job ad will not be shown.
+Not required if the link is not yet present</t>
       </text>
     </comment>
   </commentList>
@@ -91,7 +92,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>Role</t>
   </si>
@@ -108,21 +109,6 @@
     <t>PhD Student</t>
   </si>
   <si>
-    <t>ETH Zurich</t>
-  </si>
-  <si>
-    <t>Atomistic simulations of μSR spectroscopy experiments including quantum effects</t>
-  </si>
-  <si>
-    <t>Postdoc</t>
-  </si>
-  <si>
-    <t>University of Zürich UZH</t>
-  </si>
-  <si>
-    <t>Snow-coverage monitoring with cosmic muons</t>
-  </si>
-  <si>
     <t>Postdoc/Software Engineer</t>
   </si>
   <si>
@@ -132,18 +118,12 @@
     <t>Design of a secure data sharing portal for muon data</t>
   </si>
   <si>
-    <t>https://jobs.ethz.ch/job/view/JOPG_ethz_Hcey2SI</t>
-  </si>
-  <si>
     <t>https://www.psi.ch/en/hr/job-opportunities/92729-postdoctoral-data-sharing-portal</t>
   </si>
   <si>
     <t>Deadline</t>
   </si>
   <si>
-    <t>https://jobs.uzh.ch/job-vacancies/postdoctoral-fellow-in-snow-with-muons/2967a2b2cd92a0ef</t>
-  </si>
-  <si>
     <t>For any job offering, please add a row filling *all* columns</t>
   </si>
   <si>
@@ -165,7 +145,22 @@
     <t>NOTE: at the moment, the content of this file is NOT automatically mirrored to the website! You need to ask someone with permissions to apply the changes and put them online</t>
   </si>
   <si>
-    <t>is an example</t>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Giovanni Pizzi</t>
+  </si>
+  <si>
+    <t>Giovanni Pizzi (PSI), Nicola Spaldin (ETHZ)</t>
+  </si>
+  <si>
+    <t>Quantum-mechanical simulations of muons in materials</t>
+  </si>
+  <si>
+    <t>Responsible PI</t>
+  </si>
+  <si>
+    <t>Example, will be replaced</t>
   </si>
 </sst>
 </file>
@@ -173,9 +168,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -197,12 +192,6 @@
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -236,8 +225,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="169" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
@@ -587,37 +576,38 @@
   <threadedComment ref="B1" dT="2026-02-02T10:18:52.37" personId="{5C96D8BA-4A6A-AA44-843F-C7EA4DBD6FF4}" id="{3A2C8F42-915E-4B42-8C35-1087C2FD6E67}">
     <text>Please use standardized name (copy name from rows above, if one already exists)</text>
   </threadedComment>
-  <threadedComment ref="C1" dT="2026-02-02T10:19:08.34" personId="{5C96D8BA-4A6A-AA44-843F-C7EA4DBD6FF4}" id="{0DD1F034-F3C2-6143-B5EE-4D8ACB9B94D3}">
+  <threadedComment ref="D1" dT="2026-02-02T10:19:08.34" personId="{5C96D8BA-4A6A-AA44-843F-C7EA4DBD6FF4}" id="{0DD1F034-F3C2-6143-B5EE-4D8ACB9B94D3}">
     <text>Short 1-line job description</text>
   </threadedComment>
-  <threadedComment ref="D1" dT="2026-02-02T10:19:37.74" personId="{5C96D8BA-4A6A-AA44-843F-C7EA4DBD6FF4}" id="{7B781CE5-788D-EE45-89AA-868478A6290E}">
-    <text>Direct link to page with full application (and link to apply)</text>
+  <threadedComment ref="E1" dT="2026-02-02T10:19:37.74" personId="{5C96D8BA-4A6A-AA44-843F-C7EA4DBD6FF4}" id="{7B781CE5-788D-EE45-89AA-868478A6290E}">
+    <text>Direct link to page with full application (and link to apply). If not present, the button will not be shown</text>
   </threadedComment>
-  <threadedComment ref="F1" dT="2026-02-02T10:24:45.61" personId="{5C96D8BA-4A6A-AA44-843F-C7EA4DBD6FF4}" id="{86A3B50E-CB66-3648-8FB2-14FCD24209F5}">
-    <text>If the value is "TRUE", it will not be shown on the website</text>
+  <threadedComment ref="F1" dT="2026-02-05T22:35:50.45" personId="{5C96D8BA-4A6A-AA44-843F-C7EA4DBD6FF4}" id="{803435A0-8165-0344-9437-CCA1C17B6D10}">
+    <text>When the date is in the past, the job ad will not be shown.
+Not required if the link is not yet present</text>
   </threadedComment>
 </ThreadedComments>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66E7D654-8566-4343-917D-3D2DB68479B8}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="23.83203125" customWidth="1"/>
-    <col min="2" max="2" width="23.5" customWidth="1"/>
-    <col min="3" max="3" width="81.33203125" customWidth="1"/>
-    <col min="4" max="4" width="82.6640625" customWidth="1"/>
-    <col min="5" max="5" width="12.1640625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="13" customWidth="1"/>
+    <col min="2" max="3" width="23.5" customWidth="1"/>
+    <col min="4" max="4" width="81.33203125" customWidth="1"/>
+    <col min="5" max="5" width="82.6640625" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="44.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -625,86 +615,65 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="4">
+        <v>46143</v>
+      </c>
+      <c r="G2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="4">
-        <v>46143</v>
-      </c>
-      <c r="F2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
       <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="4">
-        <v>46174</v>
-      </c>
-      <c r="F3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="4">
-        <v>46204</v>
-      </c>
-      <c r="F4" t="b">
-        <v>1</v>
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{8AB2C6DF-6D21-D843-9899-4A075E71408D}"/>
-    <hyperlink ref="D4" r:id="rId2" xr:uid="{22118BF7-2732-1740-9DA3-5393C437A502}"/>
-    <hyperlink ref="D3" r:id="rId3" xr:uid="{4661B481-37EF-C241-B846-2C9AE25F490F}"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{22118BF7-2732-1740-9DA3-5393C437A502}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -723,37 +692,37 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>